<commit_message>
modifications devis et facture. Création avoir. Modification et création des pdf devis, factures, avoirs, acomptes
</commit_message>
<xml_diff>
--- a/.temp/heures.xlsx
+++ b/.temp/heures.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Semaine 11 au 17 Mai</t>
   </si>
@@ -58,7 +58,25 @@
     <t>Travail effectué</t>
   </si>
   <si>
-    <t>Modification Adresse client (Adresse, adresse2 (facultatif), adresse3 (facultatif), code postal, ville). Ajout Société et numéro de TVA pour les pros.</t>
+    <t>14:06 - 14:33 / 19:07 - 20:48</t>
+  </si>
+  <si>
+    <t>Modification Adresse client (Adresse, adresse2 (facultatif), adresse3 (facultatif), code postal, ville). Ajout Société et numéro de TVA pour les pros. Modification des répercution dans estimations, clients, devis, factures</t>
+  </si>
+  <si>
+    <t>11h37</t>
+  </si>
+  <si>
+    <t>12:05 - 12:35</t>
+  </si>
+  <si>
+    <t>Modification pdf devis et factures pour les nouvelles infos à faire figurer dessus</t>
+  </si>
+  <si>
+    <t>9h22</t>
+  </si>
+  <si>
+    <t>Modification pdf devis et factures. Modifications js pages devis spécifique et factures. Création pdf avoir et acompte ainsi que le backend de factures, devis, avoirs</t>
   </si>
 </sst>
 </file>
@@ -401,14 +419,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="128.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -425,10 +446,10 @@
         <v>9</v>
       </c>
       <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
       </c>
       <c r="E2" t="s">
         <v>12</v>
@@ -444,19 +465,50 @@
       <c r="B3" s="1">
         <v>0.36458333333333331</v>
       </c>
+      <c r="C3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.9375</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="F3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" s="1">
+        <v>0.36319444444444443</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.77430555555555547</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
+      <c r="B5" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="C5" s="1"/>
+      <c r="F5" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -467,6 +519,7 @@
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -477,6 +530,9 @@
       <c r="A9" t="s">
         <v>7</v>
       </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Modification factures et pdf factures pour relance
</commit_message>
<xml_diff>
--- a/.temp/heures.xlsx
+++ b/.temp/heures.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Semaine 11 au 17 Mai</t>
   </si>
@@ -77,6 +77,9 @@
   </si>
   <si>
     <t>Modification pdf devis et factures. Modifications js pages devis spécifique et factures. Création pdf avoir et acompte ainsi que le backend de factures, devis, avoirs</t>
+  </si>
+  <si>
+    <t>9h00</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,6 +509,12 @@
         <v>0.375</v>
       </c>
       <c r="C5" s="1"/>
+      <c r="D5" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
       <c r="F5" t="s">
         <v>20</v>
       </c>
@@ -513,6 +522,9 @@
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.375</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modifications front pour menu de gauche + ajout exemple facture relance
</commit_message>
<xml_diff>
--- a/.temp/heures.xlsx
+++ b/.temp/heures.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Semaine 11 au 17 Mai</t>
   </si>
@@ -80,6 +80,9 @@
   </si>
   <si>
     <t>9h00</t>
+  </si>
+  <si>
+    <t>Modifications pour relance facture et pdf relance facture</t>
   </si>
 </sst>
 </file>
@@ -425,7 +428,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -526,6 +529,9 @@
       <c r="B6" s="1">
         <v>0.375</v>
       </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">

</xml_diff>

<commit_message>
Ajout de la carte
</commit_message>
<xml_diff>
--- a/.temp/heures.xlsx
+++ b/.temp/heures.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Semaine 11 au 17 Mai</t>
   </si>
@@ -82,7 +82,10 @@
     <t>9h00</t>
   </si>
   <si>
-    <t>Modifications pour relance facture et pdf relance facture</t>
+    <t>Modifications pour relance facture et pdf relance facture. Carte</t>
+  </si>
+  <si>
+    <t>12:16 - 13:45 / 18:15 - 19:25</t>
   </si>
 </sst>
 </file>
@@ -428,7 +431,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -529,6 +532,9 @@
       <c r="B6" s="1">
         <v>0.375</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="F6" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Prise en charge des erreurs 404 et ds erreurs non interceptées.
</commit_message>
<xml_diff>
--- a/.temp/heures.xlsx
+++ b/.temp/heures.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Semaine 11 au 17 Mai</t>
   </si>
@@ -82,10 +82,16 @@
     <t>9h00</t>
   </si>
   <si>
-    <t>Modifications pour relance facture et pdf relance facture. Carte</t>
-  </si>
-  <si>
     <t>12:16 - 13:45 / 18:15 - 19:25</t>
+  </si>
+  <si>
+    <t>Modifications pour relance facture et pdf relance facture.Ajout de la Carte</t>
+  </si>
+  <si>
+    <t>9h46</t>
+  </si>
+  <si>
+    <t>Gestion déconnexion. Gestion 404. Ajout Prix &amp; Options.</t>
   </si>
 </sst>
 </file>
@@ -431,7 +437,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -533,17 +539,29 @@
         <v>0.375</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.89236111111111116</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F6" t="s">
         <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
+      <c r="B7" s="1">
+        <v>0.35902777777777778</v>
+      </c>
       <c r="E7" s="1"/>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">

</xml_diff>

<commit_message>
Ajout gestion des prix et options
</commit_message>
<xml_diff>
--- a/.temp/heures.xlsx
+++ b/.temp/heures.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Semaine 11 au 17 Mai</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Gestion déconnexion. Gestion 404. Ajout Prix &amp; Options.</t>
+  </si>
+  <si>
+    <t>12:03 - 12:36</t>
   </si>
 </sst>
 </file>
@@ -437,7 +440,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,6 +561,9 @@
       <c r="B7" s="1">
         <v>0.35902777777777778</v>
       </c>
+      <c r="C7" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" t="s">
         <v>25</v>

</xml_diff>

<commit_message>
ajout double clic devisitem
</commit_message>
<xml_diff>
--- a/.temp/heures.xlsx
+++ b/.temp/heures.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
   <si>
     <t>Semaine 11 au 17 Mai</t>
   </si>
@@ -118,7 +118,13 @@
     <t>9h32</t>
   </si>
   <si>
-    <t>Agenda</t>
+    <t>7h00</t>
+  </si>
+  <si>
+    <t>Agenda, modification d'éléments mineurs détectés, devis double clic</t>
+  </si>
+  <si>
+    <t>devis double clic</t>
   </si>
 </sst>
 </file>
@@ -485,7 +491,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,13 +779,25 @@
       <c r="B15" s="2">
         <v>0.35347222222222219</v>
       </c>
+      <c r="D15" s="2">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="F15" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>3</v>
+      </c>
+      <c r="B16" s="2">
+        <v>0.3527777777777778</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
modifications des fetch pour une meilleure interraction avec l'utilisateur
</commit_message>
<xml_diff>
--- a/.temp/heures.xlsx
+++ b/.temp/heures.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="39">
   <si>
     <t>Semaine 11 au 17 Mai</t>
   </si>
@@ -125,6 +125,12 @@
   </si>
   <si>
     <t>devis double clic, corrections de bugs, devis modification ux brunch + pdf, facture modifications pour statut payée, facture gestion paiement en retard</t>
+  </si>
+  <si>
+    <t>12:47 - 15:00</t>
+  </si>
+  <si>
+    <t>9h09</t>
   </si>
 </sst>
 </file>
@@ -491,7 +497,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,26 +802,38 @@
       <c r="B16" s="2">
         <v>0.3527777777777778</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.82638888888888884</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="F16" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>0.36874999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>7</v>
       </c>

</xml_diff>